<commit_message>
version final runs has added
</commit_message>
<xml_diff>
--- a/version 03/input_output/input.xlsx
+++ b/version 03/input_output/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Artificial Bee Colony\Implementation\Knapsack\knapsackProblem_Classic_ABC\version 03\input_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0786BE46-631A-4E86-A71E-1B044B9FFFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081DD5DD-B620-40E4-B8AC-18B585B04BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A572E783-3D6C-4728-9EDE-E61D3E589CC8}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,10 +514,10 @@
         <v>11</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -552,10 +552,10 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -593,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F4">
         <v>100</v>
@@ -631,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F7">
         <v>100</v>
@@ -745,7 +745,7 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F8">
         <v>100</v>
@@ -783,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -821,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F10">
         <v>100</v>
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="F11">
         <v>100</v>

</xml_diff>